<commit_message>
Update with iss position program
</commit_message>
<xml_diff>
--- a/direction_calculator/Calculations/Geocentric_Radius.xlsx
+++ b/direction_calculator/Calculations/Geocentric_Radius.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathilde Rossier\Documents\SYND1\SSC_CH\ISS-pointer\direction_calculator\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5036B4B0-CAB8-41E4-A0C1-57324288BCD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742FCAA3-2286-4690-936B-CB8664C6FF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08594BDB-5DE9-4DB2-8633-414EDF9AC49F}"/>
   </bookViews>
@@ -135,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -146,8 +146,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -170,23 +176,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>163285</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:rowOff>10885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>777735</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>30589</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>522513</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
+        <xdr:cNvPr id="4" name="Image 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C4FAB21-9A9B-493E-BC0E-3A281A3F5E97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22E7E6D6-BC76-4E11-9EFF-E9C24851AEE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -194,16 +200,21 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="6127" t="10998" r="20612" b="38327"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="830580" y="967740"/>
-          <a:ext cx="5715495" cy="1257409"/>
+          <a:off x="8327571" y="936171"/>
+          <a:ext cx="6716485" cy="3516086"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -512,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392FD6B9-2061-4C86-85F5-2D5C2C3E97C7}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -525,61 +536,61 @@
     <col min="4" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="1:15">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="2:15" ht="28.8">
-      <c r="B2" s="1" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" s="3" customFormat="1" ht="28.8">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="1:15">
       <c r="B3" s="2">
         <v>6356.7520000000004</v>
       </c>
@@ -625,146 +636,146 @@
         <v>6367030.371244451</v>
       </c>
     </row>
-    <row r="14" spans="2:15">
-      <c r="B14" s="3" t="s">
+    <row r="6" spans="1:15">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="C6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="2:15">
-      <c r="B15" s="1" t="s">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C7" s="1">
         <f>F3</f>
         <v>0.97302105798683869</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F7" s="1">
         <f>L3</f>
         <v>0.80686571319697853</v>
       </c>
     </row>
-    <row r="16" spans="2:15">
-      <c r="B16" s="1" t="s">
+    <row r="8" spans="1:15">
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C8" s="1">
         <f>RADIANS(37.62)</f>
         <v>0.65659286460026678</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F8" s="1">
         <f>RADIANS(7.35)</f>
         <v>0.12828170002158321</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="B17" s="1" t="s">
+    <row r="9" spans="1:15">
+      <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C9" s="1">
         <f>I3</f>
         <v>6363564.6064720461</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F9" s="1">
         <f>O3</f>
         <v>6367030.371244451</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="4" t="s">
+    <row r="10" spans="1:15">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="1">
-        <f>SQRT(C17^2-C20^2)*COS(C16)</f>
+      <c r="C10" s="1">
+        <f>SQRT(C9^2-C12^2)*COS(C8)</f>
         <v>2836779.2401990672</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="1">
-        <f>SQRT(F17^2-F20^2)*COS(F16)</f>
+      <c r="F10" s="1">
+        <f>SQRT(F9^2-F12^2)*COS(F8)</f>
         <v>4368298.9237109385</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1" t="s">
+    <row r="11" spans="1:15">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="1">
-        <f>SQRT(C17^2-C20^2)*SIN(C16)</f>
+      <c r="C11" s="1">
+        <f>SQRT(C9^2-C12^2)*SIN(C8)</f>
         <v>2186192.0186511232</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="1">
-        <f>SQRT(F17^2-F20^2)*SIN(F16)</f>
+      <c r="F11" s="1">
+        <f>SQRT(F9^2-F12^2)*SIN(F8)</f>
         <v>563467.04948972573</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="1">
-        <f>SQRT(F18^2+F19^2+F20^2)</f>
+      <c r="I11" s="1">
+        <f>SQRT(F10^2+F11^2+F12^2)</f>
         <v>6367030.3712444501</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1" t="s">
+    <row r="12" spans="1:15">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="1">
-        <f>C17*SIN(C15)</f>
+      <c r="C12" s="1">
+        <f>C9*SIN(C7)</f>
         <v>5260057.2716183858</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="1">
-        <f>F17*SIN(F15)</f>
+      <c r="F12" s="1">
+        <f>F9*SIN(F7)</f>
         <v>4597776.108684985</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="1">
-        <f>I19-F17</f>
+      <c r="I12" s="1">
+        <f>I11-F9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="B23" s="1" t="s">
+    <row r="15" spans="1:15">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="1">
-        <f>SQRT(C18^2+C19^2+C20^2)</f>
+      <c r="C15" s="1">
+        <f>SQRT(C10^2+C11^2+C12^2)</f>
         <v>6363564.6064720461</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="B24" s="1" t="s">
+    <row r="16" spans="1:15">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="1">
-        <f>C23-C17</f>
+      <c r="C16" s="1">
+        <f>C15-C9</f>
         <v>0</v>
       </c>
     </row>
@@ -772,9 +783,9 @@
   <mergeCells count="5">
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="K1:O1"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Presentation and last updates
</commit_message>
<xml_diff>
--- a/direction_calculator/Calculations/Geocentric_Radius.xlsx
+++ b/direction_calculator/Calculations/Geocentric_Radius.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathilde Rossier\Documents\SYND1\SSC_CH\ISS-pointer\direction_calculator\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742FCAA3-2286-4690-936B-CB8664C6FF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCC0601-593D-4143-8FCC-0CA3ED74E7B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08594BDB-5DE9-4DB2-8633-414EDF9AC49F}"/>
   </bookViews>
@@ -147,13 +147,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -176,16 +176,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>163285</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>10885</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>65315</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>522513</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -213,7 +213,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8327571" y="936171"/>
+          <a:off x="1839686" y="2677886"/>
           <a:ext cx="6716485" cy="3516086"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -526,31 +526,44 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="1"/>
-    <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="6.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="1"/>
+    <col min="7" max="7" width="6.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" s="3" customFormat="1" ht="28.8">
       <c r="B2" s="3" t="s">
@@ -637,24 +650,24 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1">
         <f>F3</f>
         <v>0.97302105798683869</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="1">
@@ -663,14 +676,14 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1">
         <f>RADIANS(37.62)</f>
         <v>0.65659286460026678</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="1">
@@ -679,14 +692,14 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="1">
         <f>I3</f>
         <v>6363564.6064720461</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="1">
@@ -695,17 +708,17 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1">
         <f>SQRT(C9^2-C12^2)*COS(C8)</f>
         <v>2836779.2401990672</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="1">
@@ -714,15 +727,15 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1">
         <f>SQRT(C9^2-C12^2)*SIN(C8)</f>
         <v>2186192.0186511232</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="1">
@@ -738,15 +751,15 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="1">
         <f>C9*SIN(C7)</f>
         <v>5260057.2716183858</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="1">
@@ -788,6 +801,7 @@
     <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>